<commit_message>
Added treeview - needs more work.
</commit_message>
<xml_diff>
--- a/docs/Grading_Guide.xlsx
+++ b/docs/Grading_Guide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/intellijProjects/ViennaUBhan/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/intellijProjects/ViennaUBahn/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF01A1DC-C977-4DB1-BB75-3112E0D2BF45}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{381EAA35-41F0-4F93-A76B-7BF6B76DA032}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
+    <workbookView xWindow="750" yWindow="1170" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Scoring</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Waypoint Support in Dijkstras ?</t>
   </si>
   <si>
-    <t>Waypoint Support in Dijkstras lowest cost?</t>
-  </si>
-  <si>
     <t>Avoiding Specified Stations in BFS</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>Avoiding Specified Stations in Dijkstras ?</t>
-  </si>
-  <si>
-    <t>Avoiding Specified Stations in Dijkstras lowest cost?</t>
   </si>
 </sst>
 </file>
@@ -301,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -379,37 +373,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -488,6 +459,32 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -577,10 +574,6 @@
 </FeaturePropertyBags>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -646,13 +639,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D33" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{898160EA-F5AD-461E-BFC7-D7BA077FCB15}" name="Scoring" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C89D5441-0C13-43BE-9ED8-65D19763A7D2}" name="Available %" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C7B0258F-D35C-4C42-AE14-919E3F617D9B}" name="Attempted?" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3C10293A-6E49-441C-928D-0EA574C2494D}" name="Potential Score" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{898160EA-F5AD-461E-BFC7-D7BA077FCB15}" name="Scoring" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C89D5441-0C13-43BE-9ED8-65D19763A7D2}" name="Available %" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C7B0258F-D35C-4C42-AE14-919E3F617D9B}" name="Attempted?" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{3C10293A-6E49-441C-928D-0EA574C2494D}" name="Potential Score" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -978,7 +971,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1057,11 +1050,11 @@
         <v>10</v>
       </c>
       <c r="C5" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1069,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,11 +1141,11 @@
         <v>5</v>
       </c>
       <c r="C14" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,7 +1161,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,17 +1169,13 @@
         <v>28</v>
       </c>
       <c r="C17" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="A18" s="13"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="17" t="b">
-        <v>0</v>
-      </c>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -1205,7 +1194,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="16" t="b">
         <v>0</v>
@@ -1213,7 +1202,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="16" t="b">
         <v>0</v>
@@ -1221,16 +1210,14 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="A23" s="13"/>
       <c r="B23" s="14"/>
       <c r="C23" s="17" t="b">
         <v>0</v>
@@ -1241,7 +1228,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,7 +1236,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,7 +1244,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1265,7 +1252,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1343,7 +1330,7 @@
       </c>
       <c r="D33" s="4">
         <f>SUM(D2:D32)</f>
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added line change penalties - buggy
</commit_message>
<xml_diff>
--- a/docs/Grading_Guide.xlsx
+++ b/docs/Grading_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/intellijProjects/ViennaUBahn/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{381EAA35-41F0-4F93-A76B-7BF6B76DA032}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAD5BE2C-441F-44A3-BA74-955336CD95AC}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="1170" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
+    <workbookView xWindow="13785" yWindow="825" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,6 +572,10 @@
     </a>
   </bag>
 </FeaturePropertyBags>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -971,7 +975,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1086,11 +1090,11 @@
         <v>10</v>
       </c>
       <c r="C9" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1102,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,7 +1110,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1115,7 +1119,7 @@
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1330,7 +1334,7 @@
       </c>
       <c r="D33" s="4">
         <f>SUM(D2:D32)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before fix map plotting - dijkstras
</commit_message>
<xml_diff>
--- a/docs/Grading_Guide.xlsx
+++ b/docs/Grading_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/intellijProjects/ViennaUBahn/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAD5BE2C-441F-44A3-BA74-955336CD95AC}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43C590A4-CDEB-4465-BCC5-CBE10436B7BE}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="825" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
+    <workbookView xWindow="13740" yWindow="915" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Scoring</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Avoiding Specified Stations in Dijkstras ?</t>
+  </si>
+  <si>
+    <t>Actual grade</t>
+  </si>
+  <si>
+    <t>Attempted</t>
   </si>
 </sst>
 </file>
@@ -295,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,6 +381,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D33" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D34" xr:uid="{38DDF248-A53C-44A5-9DD2-479F3E9B9338}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{898160EA-F5AD-461E-BFC7-D7BA077FCB15}" name="Scoring" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{C89D5441-0C13-43BE-9ED8-65D19763A7D2}" name="Available %" dataDxfId="2"/>
@@ -972,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C04D9B-956A-4B41-8C14-D88D6E479C1C}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1039,11 +1057,11 @@
         <v>10</v>
       </c>
       <c r="C4" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1327,14 +1345,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <f>SUM(B2:B32)</f>
         <v>100</v>
       </c>
+      <c r="C33" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="4">
         <f>SUM(D2:D32)</f>
-        <v>75</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="C34" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="20">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submitted for grading. 81%. Updated readme.md
</commit_message>
<xml_diff>
--- a/docs/Grading_Guide.xlsx
+++ b/docs/Grading_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/intellijProjects/ViennaUBahn/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43C590A4-CDEB-4465-BCC5-CBE10436B7BE}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{8ED74AA5-9593-4311-A74C-7311946FE651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC7411C3-BD92-423A-8D0A-A40262C43D40}"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="915" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
+    <workbookView xWindow="11985" yWindow="0" windowWidth="13275" windowHeight="13845" xr2:uid="{A9E56437-9446-4EF9-B0B1-31D2AF955185}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -993,7 +993,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1364,7 @@
         <v>32</v>
       </c>
       <c r="D34" s="20">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>